<commit_message>
Add the script for merging clinical data of BIDS compliant datasets
</commit_message>
<xml_diff>
--- a/clinica/bids/data/clinical_specifications.xlsx
+++ b/clinica/bids/data/clinical_specifications.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-33600" yWindow="-3520" windowWidth="33600" windowHeight="19240" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-64120" yWindow="-4540" windowWidth="33600" windowHeight="19240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="participant.tsv" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="190">
   <si>
     <t>Field</t>
   </si>
@@ -504,9 +504,6 @@
     <t>inclusion_date</t>
   </si>
   <si>
-    <t>parent_transmitting_fdt</t>
-  </si>
-  <si>
     <t>parent_transmitting_als</t>
   </si>
   <si>
@@ -619,6 +616,9 @@
   </si>
   <si>
     <t>SCORE BREF</t>
+  </si>
+  <si>
+    <t>parent_transmitting_ftd</t>
   </si>
 </sst>
 </file>
@@ -1691,6 +1691,108 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1498600</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1498600</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1959,8 +2061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH1017"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2011,7 +2113,7 @@
         <v>51</v>
       </c>
       <c r="K1" s="18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="L1" s="18" t="s">
         <v>3</v>
@@ -2035,7 +2137,7 @@
         <v>125</v>
       </c>
       <c r="L2" s="22" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:34" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2141,7 +2243,7 @@
     </row>
     <row r="6" spans="1:34" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
@@ -2154,13 +2256,13 @@
         <v>138</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K6" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="L6" s="17" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:34" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2229,7 +2331,7 @@
         <v>75</v>
       </c>
       <c r="K8" s="22" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="L8" s="22" t="s">
         <v>76</v>
@@ -2259,7 +2361,7 @@
         <v>141</v>
       </c>
       <c r="I9" s="17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J9" s="22" t="s">
         <v>80</v>
@@ -2318,7 +2420,7 @@
         <v>126</v>
       </c>
       <c r="L11" s="22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="12" spans="1:34" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2438,7 +2540,7 @@
         <v>108</v>
       </c>
       <c r="K18" s="22" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="L18" s="22" t="s">
         <v>109</v>
@@ -2455,13 +2557,13 @@
         <v>138</v>
       </c>
       <c r="J19" s="17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K19" s="17" t="s">
         <v>126</v>
       </c>
       <c r="L19" s="17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="20" spans="1:34" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2519,10 +2621,10 @@
         <v>138</v>
       </c>
       <c r="J23" s="17" t="s">
-        <v>151</v>
+        <v>189</v>
       </c>
       <c r="K23" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="L23" s="17" t="s">
         <v>85</v>
@@ -2541,10 +2643,10 @@
         <v>138</v>
       </c>
       <c r="J24" s="17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K24" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="L24" s="17" t="s">
         <v>85</v>
@@ -2584,7 +2686,7 @@
         <v>138</v>
       </c>
       <c r="J25" s="17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K25" s="17" t="s">
         <v>125</v>
@@ -2605,13 +2707,13 @@
         <v>138</v>
       </c>
       <c r="J26" s="17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K26" s="17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L26" s="17" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="27" spans="1:34" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2621,19 +2723,19 @@
       <c r="E28" s="22"/>
       <c r="F28" s="22"/>
       <c r="H28" s="17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I28" s="17" t="s">
         <v>138</v>
       </c>
       <c r="J28" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K28" s="17" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="L28" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="29" spans="1:34" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2642,13 +2744,13 @@
       <c r="E29" s="22"/>
       <c r="F29" s="22"/>
       <c r="H29" s="17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I29" s="17" t="s">
         <v>138</v>
       </c>
       <c r="J29" s="17" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="30" spans="1:34" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2657,13 +2759,13 @@
       <c r="E30" s="22"/>
       <c r="F30" s="22"/>
       <c r="H30" s="17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I30" s="17" t="s">
         <v>138</v>
       </c>
       <c r="J30" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="31" spans="1:34" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2672,13 +2774,13 @@
       <c r="E31" s="22"/>
       <c r="F31" s="22"/>
       <c r="H31" s="17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I31" s="17" t="s">
         <v>138</v>
       </c>
       <c r="J31" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K31" s="17" t="s">
         <v>126</v>
@@ -2690,16 +2792,16 @@
       <c r="E32" s="22"/>
       <c r="F32" s="22"/>
       <c r="H32" s="17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I32" s="17" t="s">
         <v>138</v>
       </c>
       <c r="J32" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K32" s="17" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="33" spans="1:34" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -7745,10 +7847,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7756,13 +7858,13 @@
     <col min="1" max="1" width="23.1640625" customWidth="1"/>
     <col min="2" max="2" width="44.83203125" customWidth="1"/>
     <col min="3" max="3" width="51.6640625" style="8" customWidth="1"/>
-    <col min="6" max="6" width="14.5" style="9"/>
-    <col min="7" max="7" width="20.1640625" style="9" customWidth="1"/>
-    <col min="8" max="8" width="21.5" customWidth="1"/>
-    <col min="9" max="9" width="23.5" customWidth="1"/>
+    <col min="6" max="7" width="14.5" style="9"/>
+    <col min="8" max="8" width="20.1640625" style="9" customWidth="1"/>
+    <col min="9" max="9" width="21.5" customWidth="1"/>
+    <col min="10" max="10" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -7779,22 +7881,25 @@
         <v>2</v>
       </c>
       <c r="F1" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="7"/>
       <c r="K1" s="7"/>
       <c r="L1" s="7"/>
-    </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M1" s="7"/>
+    </row>
+    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -7804,14 +7909,15 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2"/>
+      <c r="I2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -7821,11 +7927,12 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="2"/>
+      <c r="I3" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -7835,154 +7942,168 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="2"/>
+      <c r="I4" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D5" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="2"/>
+      <c r="I5" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D6" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="2"/>
+      <c r="I6" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D7" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="2"/>
+      <c r="I7" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D8" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="2"/>
+      <c r="I8" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D9" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="2"/>
+      <c r="I9" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D10" s="2" t="s">
         <v>28</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="2"/>
+      <c r="I10" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D11" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="2"/>
+      <c r="I11" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D12" s="2" t="s">
         <v>32</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="2"/>
+      <c r="I12" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D13" s="2" t="s">
         <v>34</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="2" t="s">
+      <c r="H13" s="2"/>
+      <c r="I13" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D14" s="2" t="s">
         <v>35</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="2"/>
+      <c r="I14" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D15" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
-      <c r="H15" s="2" t="s">
+      <c r="H15" s="2"/>
+      <c r="I15" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D16" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
-      <c r="H16" s="2" t="s">
+      <c r="H16" s="2"/>
+      <c r="I16" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D17" s="2" t="s">
         <v>41</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-      <c r="H17" s="2" t="s">
+      <c r="H17" s="2"/>
+      <c r="I17" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>43</v>
       </c>
@@ -7992,11 +8113,12 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
-      <c r="H18" s="2" t="s">
+      <c r="H18" s="2"/>
+      <c r="I18" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>46</v>
       </c>
@@ -8008,11 +8130,12 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
-      <c r="H19" s="2" t="s">
+      <c r="H19" s="2"/>
+      <c r="I19" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="8"/>
       <c r="B20" s="10" t="s">
         <v>119</v>
@@ -8022,14 +8145,14 @@
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
-      <c r="H20" s="8" t="s">
+      <c r="I20" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="I20" s="8" t="s">
+      <c r="J20" s="8" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="8"/>
       <c r="B21" s="11" t="s">
         <v>120</v>
@@ -8039,14 +8162,14 @@
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
-      <c r="H21" s="8" t="s">
+      <c r="I21" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="I21" s="8" t="s">
+      <c r="J21" s="8" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="8"/>
       <c r="B22" s="8" t="s">
         <v>113</v>
@@ -8056,100 +8179,100 @@
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
-      <c r="H22" s="8" t="s">
+      <c r="I22" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="I22" s="8" t="s">
+      <c r="J22" s="8" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="F23" s="9" t="s">
+    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G23" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="I23" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="9"/>
+      <c r="G24" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="G23" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="H23" t="s">
+      <c r="H24" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="I24" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="9"/>
-      <c r="F24" s="9" t="s">
+    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="9"/>
+      <c r="G25" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="G24" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="H24" t="s">
+      <c r="H25" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="I25" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="9"/>
-      <c r="F25" s="9" t="s">
+    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="9"/>
+      <c r="G26" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="G25" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="H25" t="s">
+      <c r="H26" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="I26" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="9"/>
-      <c r="F26" s="9" t="s">
+    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="9"/>
+      <c r="G27" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="G26" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="H26" t="s">
+      <c r="H27" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="I27" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="9"/>
+      <c r="G28" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="I28" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="9"/>
+      <c r="G29" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="H29" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="I29" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="9"/>
-      <c r="F27" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="G27" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="H27" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="9"/>
-      <c r="F28" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="G28" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="H28" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="9"/>
-      <c r="F29" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="G29" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="H29" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="9"/>
     </row>
-    <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="9"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix some minor problems with the conversion of clinical data for prevdemals_to_bids
</commit_message>
<xml_diff>
--- a/clinica/bids/data/clinical_specifications.xlsx
+++ b/clinica/bids/data/clinical_specifications.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-64120" yWindow="-4540" windowWidth="33600" windowHeight="19240" tabRatio="500"/>
+    <workbookView xWindow="-67200" yWindow="-4540" windowWidth="33600" windowHeight="19240" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="participant.tsv" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="190">
   <si>
     <t>Field</t>
   </si>
@@ -1793,6 +1793,57 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1498600</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2061,7 +2112,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH1017"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
@@ -8282,23 +8333,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="23.83203125" customWidth="1"/>
-    <col min="4" max="4" width="36.6640625" customWidth="1"/>
+    <col min="4" max="4" width="22.5" customWidth="1"/>
     <col min="5" max="5" width="19.6640625" customWidth="1"/>
     <col min="6" max="6" width="21.1640625" customWidth="1"/>
-    <col min="8" max="8" width="21.6640625" customWidth="1"/>
-    <col min="9" max="9" width="21.1640625" customWidth="1"/>
+    <col min="7" max="8" width="21.1640625" style="9" customWidth="1"/>
+    <col min="10" max="10" width="21.6640625" customWidth="1"/>
+    <col min="11" max="11" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -8316,39 +8368,47 @@
         <v>121</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>51</v>
+        <v>135</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="I1" s="13" t="s">
         <v>51</v>
       </c>
       <c r="J1" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="L1" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="K1" s="12"/>
-    </row>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M1" s="12"/>
+    </row>
+    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12" t="s">
+      <c r="J2" s="12"/>
+      <c r="K2" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="L2" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="K2" s="12"/>
-    </row>
-    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M2" s="12"/>
+    </row>
+    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12"/>
       <c r="B3" s="12"/>
       <c r="C3" s="12" t="s">
@@ -8357,19 +8417,21 @@
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
-      <c r="G3" s="12" t="s">
-        <v>6</v>
-      </c>
+      <c r="G3" s="12"/>
       <c r="H3" s="12"/>
       <c r="I3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="L3" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="K3" s="12"/>
-    </row>
-    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M3" s="12"/>
+    </row>
+    <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>127</v>
       </c>
@@ -8382,21 +8444,23 @@
       <c r="F4" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="J4" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="K4" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="L4" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="K4" s="12"/>
-    </row>
-    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M4" s="12"/>
+    </row>
+    <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>132</v>
       </c>
@@ -8409,19 +8473,21 @@
       <c r="F5" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="J5" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="K5" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="L5" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="K5" s="12"/>
+      <c r="M5" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Create scans files for insight_to_bids converter
</commit_message>
<xml_diff>
--- a/clinica/bids/data/clinical_specifications.xlsx
+++ b/clinica/bids/data/clinical_specifications.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-67200" yWindow="-4540" windowWidth="33600" windowHeight="19240" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-32160" yWindow="-3840" windowWidth="33600" windowHeight="14620" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="participant.tsv" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="191">
   <si>
     <t>Field</t>
   </si>
@@ -619,6 +619,9 @@
   </si>
   <si>
     <t>parent_transmitting_ftd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                              </t>
   </si>
 </sst>
 </file>
@@ -1844,6 +1847,57 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1498600</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2112,8 +2166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH1017"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8333,24 +8387,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="23.83203125" customWidth="1"/>
-    <col min="4" max="4" width="22.5" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" customWidth="1"/>
-    <col min="6" max="6" width="21.1640625" customWidth="1"/>
-    <col min="7" max="8" width="21.1640625" style="9" customWidth="1"/>
-    <col min="10" max="10" width="21.6640625" customWidth="1"/>
-    <col min="11" max="11" width="21.1640625" customWidth="1"/>
+    <col min="3" max="3" width="14.5" style="9"/>
+    <col min="5" max="5" width="22.5" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" customWidth="1"/>
+    <col min="7" max="7" width="21.1640625" customWidth="1"/>
+    <col min="8" max="9" width="21.1640625" style="9" customWidth="1"/>
+    <col min="11" max="11" width="21.6640625" customWidth="1"/>
+    <col min="12" max="12" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -8358,136 +8413,145 @@
         <v>110</v>
       </c>
       <c r="C1" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="12"/>
+      <c r="F1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="I1" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="J1" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="L1" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="M1" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="M1" s="12"/>
-    </row>
-    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N1" s="12"/>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="D2" s="12" t="s">
+        <v>190</v>
+      </c>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="12"/>
+      <c r="J2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12" t="s">
+      <c r="K2" s="12"/>
+      <c r="L2" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="M2" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="M2" s="12"/>
-    </row>
-    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N2" s="12"/>
+    </row>
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12"/>
       <c r="B3" s="12"/>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="12"/>
+      <c r="D3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="12"/>
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="12"/>
+      <c r="J3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="12"/>
+      <c r="L3" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="M3" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="M3" s="12"/>
-    </row>
-    <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N3" s="12"/>
+    </row>
+    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>127</v>
       </c>
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="12"/>
+      <c r="F4" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="G4" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="G4" s="12"/>
       <c r="H4" s="12"/>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="12"/>
+      <c r="J4" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="K4" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="K4" s="12" t="s">
+      <c r="L4" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="L4" s="12" t="s">
+      <c r="M4" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="M4" s="12"/>
-    </row>
-    <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N4" s="12"/>
+    </row>
+    <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>132</v>
       </c>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="12"/>
+      <c r="F5" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="G5" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="G5" s="12"/>
       <c r="H5" s="12"/>
-      <c r="I5" s="12" t="s">
+      <c r="I5" s="12"/>
+      <c r="J5" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="K5" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="K5" s="12" t="s">
+      <c r="L5" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="L5" s="12" t="s">
+      <c r="M5" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update the list of clinical data to convert for insight_to_bids
</commit_message>
<xml_diff>
--- a/clinica/bids/data/clinical_specifications.xlsx
+++ b/clinica/bids/data/clinical_specifications.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-32160" yWindow="-3840" windowWidth="33600" windowHeight="14620" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-33600" yWindow="-2400" windowWidth="33600" windowHeight="15540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="participant.tsv" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="220">
   <si>
     <t>Field</t>
   </si>
@@ -387,9 +387,6 @@
     <t>PAT_EDUCATION</t>
   </si>
   <si>
-    <t>Analyses_INSIGHT_M0_20151201/Analyses_HPC_SACHA</t>
-  </si>
-  <si>
     <t>volume (cm3)</t>
   </si>
   <si>
@@ -405,9 +402,6 @@
     <t>cati_whasa_volume</t>
   </si>
   <si>
-    <t>Analyses_INSIGHT_M0_20151201/Analyses_HPC_WHASA</t>
-  </si>
-  <si>
     <t>vol_left_hippocampus (cm3)</t>
   </si>
   <si>
@@ -622,13 +616,107 @@
   </si>
   <si>
     <t xml:space="preserve">                              </t>
+  </si>
+  <si>
+    <t>rh_MeanThickness_thickness (mm)</t>
+  </si>
+  <si>
+    <t>freesurfer_rh_mean_thickness</t>
+  </si>
+  <si>
+    <t>lh_MeanThickness_thickness (mm)</t>
+  </si>
+  <si>
+    <t>freesurfer_lh_mean_thickness</t>
+  </si>
+  <si>
+    <t>EQ_SCORE</t>
+  </si>
+  <si>
+    <t>TST_NRO_NL.xls/EQ5D</t>
+  </si>
+  <si>
+    <t>EQ</t>
+  </si>
+  <si>
+    <t>Total Score</t>
+  </si>
+  <si>
+    <t>TST_NRO_NL.xls/SPPB</t>
+  </si>
+  <si>
+    <t>SPPB</t>
+  </si>
+  <si>
+    <t>AD8_SCORE</t>
+  </si>
+  <si>
+    <t>Tst_NRO_NP.xlsx/AD8</t>
+  </si>
+  <si>
+    <t>AD8</t>
+  </si>
+  <si>
+    <t>Tst_NRO_NP.xlsx/MCQ</t>
+  </si>
+  <si>
+    <t>MEM</t>
+  </si>
+  <si>
+    <t>AD_SCORE</t>
+  </si>
+  <si>
+    <t>AD</t>
+  </si>
+  <si>
+    <t>motivation_starkstein</t>
+  </si>
+  <si>
+    <t>Lexical Verbal Fluency Score</t>
+  </si>
+  <si>
+    <t>verbal_fluency</t>
+  </si>
+  <si>
+    <t>Analyses_INSIGHT_M0_20151201.xlsx/Analyses_thichness_Freesurfer</t>
+  </si>
+  <si>
+    <t>Analyses_INSIGHT_M0_20151201.xlsx/Analyses_HPC_SACHA</t>
+  </si>
+  <si>
+    <t>Analyses_INSIGHT_M0_20151201.xlsx/Analyses_HPC_WHASA</t>
+  </si>
+  <si>
+    <t>Tst_NRO_NP.xlsx/Starkstein</t>
+  </si>
+  <si>
+    <t>Tst_NRO_NP.xlsx/Verbal Fluency</t>
+  </si>
+  <si>
+    <t>Motivation scale</t>
+  </si>
+  <si>
+    <t>Memory Complaints Questionnaire - Recent (subject)
+MEM_SCORE</t>
+  </si>
+  <si>
+    <t>Tst_NRO_NP.xlsx/MA_NOS</t>
+  </si>
+  <si>
+    <t>SUVR</t>
+  </si>
+  <si>
+    <t>SUVr global</t>
+  </si>
+  <si>
+    <t>ANALYSE_PET_AV45.xls/Sheet 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -728,6 +816,11 @@
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -785,7 +878,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -797,8 +890,12 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -852,18 +949,26 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1898,6 +2003,57 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1498600</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2206,19 +2362,19 @@
         <v>2</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="I1" s="19" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="J1" s="18" t="s">
         <v>51</v>
       </c>
       <c r="K1" s="18" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="L1" s="18" t="s">
         <v>3</v>
@@ -2239,10 +2395,10 @@
         <v>53</v>
       </c>
       <c r="K2" s="23" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="L2" s="22" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:34" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2261,19 +2417,19 @@
         <v>57</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="I3" s="17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J3" s="22" t="s">
         <v>58</v>
       </c>
       <c r="K3" s="22" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="L3" s="17"/>
       <c r="M3" s="15"/>
@@ -2315,13 +2471,13 @@
         <v>61</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J4" s="22" t="s">
         <v>62</v>
       </c>
       <c r="K4" s="22" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="M4" s="22"/>
     </row>
@@ -2336,38 +2492,38 @@
         <v>64</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J5" s="22" t="s">
         <v>65</v>
       </c>
       <c r="K5" s="22" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="L5" s="22"/>
     </row>
     <row r="6" spans="1:34" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
       <c r="F6" s="22"/>
       <c r="H6" s="17" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="I6" s="17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="K6" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L6" s="17" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:34" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2386,22 +2542,22 @@
         <v>68</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I7" s="17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J7" s="22" t="s">
         <v>69</v>
       </c>
       <c r="K7" s="22" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="L7" s="22" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:34" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2424,19 +2580,19 @@
         <v>74</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I8" s="17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J8" s="22" t="s">
         <v>75</v>
       </c>
       <c r="K8" s="22" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L8" s="22" t="s">
         <v>76</v>
@@ -2460,19 +2616,19 @@
         <v>79</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I9" s="17" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="J9" s="22" t="s">
         <v>80</v>
       </c>
       <c r="K9" s="22" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="L9" s="22" t="s">
         <v>81</v>
@@ -2513,19 +2669,19 @@
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
       <c r="H11" s="17" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I11" s="17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J11" s="22" t="s">
         <v>88</v>
       </c>
       <c r="K11" s="22" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="L11" s="22" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:34" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2547,7 +2703,7 @@
         <v>92</v>
       </c>
       <c r="K12" s="22" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="L12" s="22" t="s">
         <v>81</v>
@@ -2578,7 +2734,7 @@
         <v>97</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J14" s="22" t="s">
         <v>98</v>
@@ -2614,7 +2770,7 @@
         <v>103</v>
       </c>
       <c r="K16" s="22" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:34" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2645,7 +2801,7 @@
         <v>108</v>
       </c>
       <c r="K18" s="22" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="L18" s="22" t="s">
         <v>109</v>
@@ -2656,30 +2812,30 @@
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
       <c r="H19" s="17" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="I19" s="17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J19" s="17" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="K19" s="17" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="L19" s="17" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="20" spans="1:34" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H20" s="17" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="I20" s="17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J20" s="17" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="21" spans="1:34" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2690,19 +2846,19 @@
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="H21" s="17" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="I21" s="17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J21" s="17" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="K21" s="17" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:34" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2720,16 +2876,16 @@
       <c r="E23" s="22"/>
       <c r="F23" s="22"/>
       <c r="H23" s="17" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="I23" s="17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J23" s="17" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="K23" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L23" s="17" t="s">
         <v>85</v>
@@ -2742,16 +2898,16 @@
       <c r="E24" s="22"/>
       <c r="F24" s="22"/>
       <c r="H24" s="17" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="I24" s="17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J24" s="17" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="K24" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L24" s="17" t="s">
         <v>85</v>
@@ -2785,16 +2941,16 @@
       <c r="E25" s="22"/>
       <c r="F25" s="22"/>
       <c r="H25" s="17" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="I25" s="17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J25" s="17" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="K25" s="17" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="L25" s="17" t="s">
         <v>81</v>
@@ -2806,19 +2962,19 @@
       <c r="E26" s="22"/>
       <c r="F26" s="22"/>
       <c r="H26" s="17" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="I26" s="17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J26" s="17" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="K26" s="17" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="L26" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="27" spans="1:34" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2828,19 +2984,19 @@
       <c r="E28" s="22"/>
       <c r="F28" s="22"/>
       <c r="H28" s="17" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="I28" s="17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J28" s="17" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K28" s="17" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="L28" s="17" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="29" spans="1:34" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2849,13 +3005,13 @@
       <c r="E29" s="22"/>
       <c r="F29" s="22"/>
       <c r="H29" s="17" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="I29" s="17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J29" s="17" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="30" spans="1:34" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2864,13 +3020,13 @@
       <c r="E30" s="22"/>
       <c r="F30" s="22"/>
       <c r="H30" s="17" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="I30" s="17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J30" s="17" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="31" spans="1:34" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2879,16 +3035,16 @@
       <c r="E31" s="22"/>
       <c r="F31" s="22"/>
       <c r="H31" s="17" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="I31" s="17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J31" s="17" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="K31" s="17" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="32" spans="1:34" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2897,16 +3053,16 @@
       <c r="E32" s="22"/>
       <c r="F32" s="22"/>
       <c r="H32" s="17" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I32" s="17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J32" s="17" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="K32" s="17" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="33" spans="1:34" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -7952,10 +8108,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7986,13 +8142,13 @@
         <v>2</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>51</v>
@@ -8243,145 +8399,304 @@
     <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="8"/>
       <c r="B20" s="10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>112</v>
+        <v>210</v>
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="I20" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="8"/>
       <c r="B21" s="11" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>112</v>
+        <v>210</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="I21" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J21" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="8"/>
       <c r="B22" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>118</v>
+        <v>211</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="I22" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="G23" s="9" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H23" s="9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="I23" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="9"/>
       <c r="G24" s="9" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="I24" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="9"/>
       <c r="G25" s="9" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="I25" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="9"/>
       <c r="G26" s="9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="H26" s="9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="I26" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="9"/>
       <c r="G27" s="9" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="I27" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="9"/>
       <c r="G28" s="9" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="I28" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="9"/>
       <c r="G29" s="9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="H29" s="9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="I29" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="9"/>
-    </row>
-    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="9"/>
+        <v>185</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="12"/>
+      <c r="B30" s="29" t="s">
+        <v>189</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="12"/>
+      <c r="B31" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="12"/>
+      <c r="B32" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="C32" s="29" t="s">
+        <v>194</v>
+      </c>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="12"/>
+      <c r="B33" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="C33" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="12"/>
+      <c r="B34" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="12"/>
+      <c r="B35" s="30" t="s">
+        <v>215</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="12"/>
+      <c r="B36" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="12"/>
+      <c r="B37" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="12"/>
+      <c r="B38" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="12" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="I39" s="12" t="s">
+        <v>217</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -8389,7 +8704,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -8423,25 +8738,25 @@
         <v>2</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="J1" s="13" t="s">
         <v>51</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="L1" s="13" t="s">
         <v>51</v>
       </c>
       <c r="M1" s="13" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="N1" s="12"/>
     </row>
@@ -8450,7 +8765,7 @@
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
@@ -8462,10 +8777,10 @@
       </c>
       <c r="K2" s="12"/>
       <c r="L2" s="12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N2" s="12"/>
     </row>
@@ -8489,67 +8804,67 @@
         <v>7</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="N3" s="12"/>
     </row>
     <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
       <c r="F4" s="12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
       <c r="J4" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="L4" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="K4" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="L4" s="12" t="s">
-        <v>131</v>
-      </c>
       <c r="M4" s="12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N4" s="12"/>
     </row>
     <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
       <c r="F5" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
       <c r="J5" s="12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="K5" s="12" t="s">
         <v>20</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N5" s="12"/>
     </row>

</xml_diff>